<commit_message>
UI integration for transaction
</commit_message>
<xml_diff>
--- a/Documentation/Database.xlsx
+++ b/Documentation/Database.xlsx
@@ -709,8 +709,8 @@
   <dimension ref="A1:XFD153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>